<commit_message>
Fix/minor change oca dew v (#130)
* Minor fix from feedback

* Added dropdown menu for entry code

* Removed any positive integer

* minor fix when clear uploaded data

* Fix a bug related to clearing and loading a new file for attribute matching

* Fixed validator parser

* Changed help storage page

* Removed unused codes
</commit_message>
<xml_diff>
--- a/dummyData/err_data_entry.xlsx
+++ b/dummyData/err_data_entry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900E368A-2AFC-A24F-BC8A-94D7BE312957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EFF901-94CE-9A4F-8402-2A92ED87DD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="19980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema Description" sheetId="1" r:id="rId1"/>
     <sheet name="Data Entry" sheetId="2" r:id="rId2"/>
-    <sheet name="Schema conformant data" sheetId="3" r:id="rId3"/>
+    <sheet name="Schema Conformant Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -737,7 +737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -1297,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>